<commit_message>
Adding RTI part 1
</commit_message>
<xml_diff>
--- a/Lab 4/control_store_lab_4.xlsx
+++ b/Lab 4/control_store_lab_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffacd89b2f1a651/Documents/Current Classes/ECE 460N/Labs/Lab 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffacd89b2f1a651/Documents/Current Classes/ECE 460N/Labs/Lab 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="894" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73DC779E-86E9-464C-B5A8-B30DBA6065B3}"/>
+  <xr:revisionPtr revIDLastSave="1033" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F9F6274-A491-4E33-A1A7-C3EF4C1C87D9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Store" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2785" uniqueCount="99">
   <si>
     <t>000000  (state 0)</t>
   </si>
@@ -296,6 +296,27 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>LD.TEMP</t>
+  </si>
+  <si>
+    <t>LD.PSR</t>
+  </si>
+  <si>
+    <t>GatePSR</t>
+  </si>
+  <si>
+    <t>MARPSR</t>
+  </si>
+  <si>
+    <t>SRSMUX</t>
+  </si>
+  <si>
+    <t>DRSMUX</t>
+  </si>
+  <si>
+    <t>ALUMUX</t>
   </si>
 </sst>
 </file>
@@ -483,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -536,6 +557,21 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="75"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,11 +887,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ65"/>
+  <dimension ref="A1:AU65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:AJ65"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -865,12 +901,15 @@
     <col min="3" max="3" width="2.453125" style="7" customWidth="1"/>
     <col min="4" max="4" width="2.453125" style="6" customWidth="1"/>
     <col min="5" max="9" width="2.453125" style="7" customWidth="1"/>
-    <col min="10" max="15" width="2.453125" style="6" customWidth="1"/>
+    <col min="10" max="13" width="2.453125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="2.453125" style="33" customWidth="1"/>
+    <col min="15" max="15" width="2.453125" style="6" customWidth="1"/>
     <col min="16" max="36" width="2.453125" style="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.1796875" style="3"/>
+    <col min="37" max="43" width="2.453125" style="3" customWidth="1"/>
+    <col min="44" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>64</v>
@@ -896,7 +935,7 @@
       <c r="M1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="28" t="s">
         <v>70</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -959,8 +998,33 @@
       <c r="AJ1" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="AK1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
     </row>
-    <row r="2" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1064,7 @@
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="29" t="s">
         <v>91</v>
       </c>
       <c r="O2" s="4" t="s">
@@ -1066,11 +1130,32 @@
       <c r="AI2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ2" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1110,7 +1195,7 @@
       <c r="M3" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O3" s="5" t="s">
@@ -1176,11 +1261,32 @@
       <c r="AI3" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ3" s="5" t="s">
+      <c r="AJ3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK3" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL3" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM3" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN3" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO3" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP3" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ3" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
@@ -1220,7 +1326,7 @@
       <c r="M4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O4" s="5" t="s">
@@ -1286,11 +1392,32 @@
       <c r="AI4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ4" s="5" t="s">
+      <c r="AJ4" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ4" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>3</v>
       </c>
@@ -1330,7 +1457,7 @@
       <c r="M5" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O5" s="5" t="s">
@@ -1396,11 +1523,32 @@
       <c r="AI5" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ5" s="5" t="s">
+      <c r="AJ5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ5" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
@@ -1440,7 +1588,7 @@
       <c r="M6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O6" s="5" t="s">
@@ -1506,11 +1654,32 @@
       <c r="AI6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ6" s="5" t="s">
+      <c r="AJ6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK6" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL6" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM6" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN6" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO6" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP6" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ6" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +1719,7 @@
       <c r="M7" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O7" s="5" t="s">
@@ -1616,11 +1785,32 @@
       <c r="AI7" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ7" s="5" t="s">
+      <c r="AJ7" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK7" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL7" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM7" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN7" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO7" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP7" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ7" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
@@ -1660,7 +1850,7 @@
       <c r="M8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O8" s="5" t="s">
@@ -1726,11 +1916,32 @@
       <c r="AI8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ8" s="5" t="s">
-        <v>90</v>
+      <c r="AJ8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ8" s="27" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>7</v>
       </c>
@@ -1770,7 +1981,7 @@
       <c r="M9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O9" s="5" t="s">
@@ -1836,11 +2047,32 @@
       <c r="AI9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ9" s="5" t="s">
-        <v>90</v>
+      <c r="AJ9" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ9" s="27" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>8</v>
       </c>
@@ -1854,13 +2086,13 @@
         <v>91</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>91</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>91</v>
@@ -1872,7 +2104,7 @@
         <v>91</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>91</v>
@@ -1880,7 +2112,7 @@
       <c r="M10" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="31" t="s">
         <v>91</v>
       </c>
       <c r="O10" s="13" t="s">
@@ -1899,7 +2131,7 @@
         <v>91</v>
       </c>
       <c r="T10" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U10" s="13" t="s">
         <v>91</v>
@@ -1932,10 +2164,10 @@
         <v>91</v>
       </c>
       <c r="AE10" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF10" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AG10" s="13" t="s">
         <v>91</v>
@@ -1946,11 +2178,32 @@
       <c r="AI10" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="AJ10" s="14" t="s">
+      <c r="AJ10" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO10" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ10" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>9</v>
       </c>
@@ -1990,7 +2243,7 @@
       <c r="M11" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O11" s="5" t="s">
@@ -2056,11 +2309,32 @@
       <c r="AI11" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ11" s="5" t="s">
+      <c r="AJ11" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ11" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>10</v>
       </c>
@@ -2100,7 +2374,7 @@
       <c r="M12" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="N12" s="31" t="s">
         <v>91</v>
       </c>
       <c r="O12" s="13" t="s">
@@ -2166,11 +2440,32 @@
       <c r="AI12" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="AJ12" s="14" t="s">
+      <c r="AJ12" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ12" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>11</v>
       </c>
@@ -2210,7 +2505,7 @@
       <c r="M13" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="N13" s="14" t="s">
+      <c r="N13" s="31" t="s">
         <v>91</v>
       </c>
       <c r="O13" s="13" t="s">
@@ -2276,11 +2571,32 @@
       <c r="AI13" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="AJ13" s="14" t="s">
+      <c r="AJ13" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ13" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>12</v>
       </c>
@@ -2320,7 +2636,7 @@
       <c r="M14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O14" s="5" t="s">
@@ -2386,11 +2702,32 @@
       <c r="AI14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ14" s="5" t="s">
+      <c r="AJ14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK14" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL14" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM14" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN14" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO14" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP14" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ14" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>13</v>
       </c>
@@ -2430,7 +2767,7 @@
       <c r="M15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O15" s="5" t="s">
@@ -2496,11 +2833,32 @@
       <c r="AI15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ15" s="5" t="s">
+      <c r="AJ15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK15" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL15" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM15" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN15" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO15" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP15" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ15" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>14</v>
       </c>
@@ -2540,7 +2898,7 @@
       <c r="M16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O16" s="5" t="s">
@@ -2606,11 +2964,32 @@
       <c r="AI16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ16" s="5" t="s">
-        <v>90</v>
+      <c r="AJ16" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ16" s="27" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>15</v>
       </c>
@@ -2650,7 +3029,7 @@
       <c r="M17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O17" s="5" t="s">
@@ -2716,11 +3095,32 @@
       <c r="AI17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ17" s="5" t="s">
+      <c r="AJ17" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ17" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>16</v>
       </c>
@@ -2760,7 +3160,7 @@
       <c r="M18" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O18" s="5" t="s">
@@ -2826,11 +3226,32 @@
       <c r="AI18" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ18" s="5" t="s">
+      <c r="AJ18" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK18" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL18" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM18" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN18" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO18" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP18" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ18" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>17</v>
       </c>
@@ -2870,7 +3291,7 @@
       <c r="M19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O19" s="5" t="s">
@@ -2936,11 +3357,32 @@
       <c r="AI19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ19" s="5" t="s">
+      <c r="AJ19" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ19" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>18</v>
       </c>
@@ -2980,7 +3422,7 @@
       <c r="M20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O20" s="5" t="s">
@@ -3046,11 +3488,32 @@
       <c r="AI20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ20" s="5" t="s">
+      <c r="AJ20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ20" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>19</v>
       </c>
@@ -3090,7 +3553,7 @@
       <c r="M21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O21" s="5" t="s">
@@ -3156,11 +3619,32 @@
       <c r="AI21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ21" s="5" t="s">
+      <c r="AJ21" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK21" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL21" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM21" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN21" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO21" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP21" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ21" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>20</v>
       </c>
@@ -3200,7 +3684,7 @@
       <c r="M22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O22" s="5" t="s">
@@ -3266,11 +3750,32 @@
       <c r="AI22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ22" s="5" t="s">
+      <c r="AJ22" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ22" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>21</v>
       </c>
@@ -3310,7 +3815,7 @@
       <c r="M23" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O23" s="5" t="s">
@@ -3376,11 +3881,32 @@
       <c r="AI23" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ23" s="5" t="s">
-        <v>90</v>
+      <c r="AJ23" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ23" s="27" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>22</v>
       </c>
@@ -3420,7 +3946,7 @@
       <c r="M24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O24" s="5" t="s">
@@ -3486,11 +4012,32 @@
       <c r="AI24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ24" s="5" t="s">
-        <v>90</v>
+      <c r="AJ24" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ24" s="27" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
         <v>23</v>
       </c>
@@ -3530,7 +4077,7 @@
       <c r="M25" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O25" s="5" t="s">
@@ -3596,11 +4143,32 @@
       <c r="AI25" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ25" s="5" t="s">
+      <c r="AJ25" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK25" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL25" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM25" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN25" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO25" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP25" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ25" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>24</v>
       </c>
@@ -3640,7 +4208,7 @@
       <c r="M26" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O26" s="5" t="s">
@@ -3706,11 +4274,32 @@
       <c r="AI26" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ26" s="5" t="s">
+      <c r="AJ26" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK26" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL26" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM26" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN26" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO26" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP26" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ26" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
         <v>25</v>
       </c>
@@ -3750,7 +4339,7 @@
       <c r="M27" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="N27" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O27" s="5" t="s">
@@ -3816,11 +4405,32 @@
       <c r="AI27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ27" s="5" t="s">
+      <c r="AJ27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK27" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL27" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM27" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN27" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO27" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP27" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ27" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -3860,7 +4470,7 @@
       <c r="M28" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N28" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O28" s="13" t="s">
@@ -3929,8 +4539,29 @@
       <c r="AJ28" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK28" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL28" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM28" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN28" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO28" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP28" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ28" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
         <v>27</v>
       </c>
@@ -3970,7 +4601,7 @@
       <c r="M29" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O29" s="5" t="s">
@@ -4036,11 +4667,32 @@
       <c r="AI29" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ29" s="5" t="s">
+      <c r="AJ29" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK29" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL29" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM29" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN29" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO29" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP29" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ29" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
         <v>28</v>
       </c>
@@ -4080,7 +4732,7 @@
       <c r="M30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N30" s="5" t="s">
+      <c r="N30" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O30" s="5" t="s">
@@ -4146,11 +4798,32 @@
       <c r="AI30" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ30" s="5" t="s">
+      <c r="AJ30" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK30" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL30" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM30" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN30" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO30" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP30" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ30" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
@@ -4190,7 +4863,7 @@
       <c r="M31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N31" s="5" t="s">
+      <c r="N31" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O31" s="5" t="s">
@@ -4256,11 +4929,32 @@
       <c r="AI31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ31" s="5" t="s">
+      <c r="AJ31" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK31" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL31" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM31" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN31" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO31" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP31" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ31" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>30</v>
       </c>
@@ -4300,7 +4994,7 @@
       <c r="M32" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N32" s="5" t="s">
+      <c r="N32" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O32" s="5" t="s">
@@ -4366,11 +5060,32 @@
       <c r="AI32" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ32" s="5" t="s">
+      <c r="AJ32" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK32" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL32" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM32" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN32" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO32" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP32" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ32" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
         <v>31</v>
       </c>
@@ -4410,7 +5125,7 @@
       <c r="M33" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N33" s="5" t="s">
+      <c r="N33" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O33" s="5" t="s">
@@ -4476,11 +5191,32 @@
       <c r="AI33" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ33" s="5" t="s">
+      <c r="AJ33" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK33" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL33" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM33" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN33" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO33" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP33" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ33" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>32</v>
       </c>
@@ -4520,7 +5256,7 @@
       <c r="M34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="N34" s="30" t="s">
         <v>90</v>
       </c>
       <c r="O34" s="5" t="s">
@@ -4586,11 +5322,32 @@
       <c r="AI34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AJ34" s="5" t="s">
+      <c r="AJ34" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK34" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL34" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM34" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN34" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO34" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP34" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ34" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
         <v>33</v>
       </c>
@@ -4630,7 +5387,7 @@
       <c r="M35" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N35" s="5" t="s">
+      <c r="N35" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O35" s="5" t="s">
@@ -4696,11 +5453,32 @@
       <c r="AI35" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ35" s="5" t="s">
+      <c r="AJ35" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK35" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL35" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM35" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN35" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO35" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP35" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ35" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
@@ -4740,7 +5518,7 @@
       <c r="M36" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N36" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O36" s="9" t="s">
@@ -4809,8 +5587,29 @@
       <c r="AJ36" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK36" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL36" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM36" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN36" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO36" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP36" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ36" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="37" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>35</v>
       </c>
@@ -4850,7 +5649,7 @@
       <c r="M37" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="N37" s="5" t="s">
+      <c r="N37" s="30" t="s">
         <v>91</v>
       </c>
       <c r="O37" s="5" t="s">
@@ -4916,11 +5715,32 @@
       <c r="AI37" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AJ37" s="5" t="s">
+      <c r="AJ37" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK37" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL37" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM37" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN37" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO37" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP37" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ37" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>36</v>
       </c>
@@ -4960,7 +5780,7 @@
       <c r="M38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N38" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O38" s="9" t="s">
@@ -5029,8 +5849,29 @@
       <c r="AJ38" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK38" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL38" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM38" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN38" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO38" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP38" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ38" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="39" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>37</v>
       </c>
@@ -5070,7 +5911,7 @@
       <c r="M39" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N39" s="9" t="s">
+      <c r="N39" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O39" s="9" t="s">
@@ -5139,8 +5980,29 @@
       <c r="AJ39" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK39" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL39" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM39" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN39" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO39" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP39" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ39" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="40" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
@@ -5180,7 +6042,7 @@
       <c r="M40" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N40" s="9" t="s">
+      <c r="N40" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O40" s="9" t="s">
@@ -5249,8 +6111,29 @@
       <c r="AJ40" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK40" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL40" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM40" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN40" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO40" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP40" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ40" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="41" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -5290,7 +6173,7 @@
       <c r="M41" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N41" s="9" t="s">
+      <c r="N41" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O41" s="9" t="s">
@@ -5359,9 +6242,30 @@
       <c r="AJ41" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK41" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL41" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM41" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN41" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO41" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP41" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ41" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="42" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
+    <row r="42" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="25" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -5371,16 +6275,16 @@
         <v>91</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>91</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>91</v>
@@ -5395,12 +6299,12 @@
         <v>91</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M42" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N42" s="9" t="s">
+      <c r="N42" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O42" s="9" t="s">
@@ -5458,19 +6362,40 @@
         <v>91</v>
       </c>
       <c r="AG42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AH42" s="9" t="s">
         <v>91</v>
       </c>
       <c r="AI42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AJ42" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK42" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL42" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM42" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN42" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO42" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP42" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ42" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="43" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>41</v>
       </c>
@@ -5510,7 +6435,7 @@
       <c r="M43" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N43" s="9" t="s">
+      <c r="N43" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O43" s="9" t="s">
@@ -5579,9 +6504,30 @@
       <c r="AJ43" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK43" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL43" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM43" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN43" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO43" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP43" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ43" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="44" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -5594,22 +6540,22 @@
         <v>91</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>91</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>91</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>91</v>
@@ -5620,7 +6566,7 @@
       <c r="M44" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N44" s="9" t="s">
+      <c r="N44" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O44" s="9" t="s">
@@ -5630,13 +6576,13 @@
         <v>91</v>
       </c>
       <c r="Q44" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R44" s="9" t="s">
         <v>91</v>
       </c>
       <c r="S44" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T44" s="9" t="s">
         <v>91</v>
@@ -5651,7 +6597,7 @@
         <v>91</v>
       </c>
       <c r="X44" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y44" s="9" t="s">
         <v>91</v>
@@ -5689,9 +6635,30 @@
       <c r="AJ44" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK44" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL44" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM44" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN44" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO44" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP44" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ44" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="45" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+    <row r="45" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="25" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
@@ -5704,16 +6671,16 @@
         <v>91</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>91</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>91</v>
@@ -5722,7 +6689,7 @@
         <v>91</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L45" s="9" t="s">
         <v>91</v>
@@ -5730,11 +6697,11 @@
       <c r="M45" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N45" s="9" t="s">
+      <c r="N45" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P45" s="9" t="s">
         <v>91</v>
@@ -5749,7 +6716,7 @@
         <v>91</v>
       </c>
       <c r="T45" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U45" s="9" t="s">
         <v>91</v>
@@ -5799,9 +6766,30 @@
       <c r="AJ45" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK45" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL45" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM45" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN45" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO45" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP45" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ45" s="27" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="46" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
@@ -5811,19 +6799,19 @@
         <v>91</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>91</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>91</v>
@@ -5835,12 +6823,12 @@
         <v>91</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M46" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N46" s="9" t="s">
+      <c r="N46" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O46" s="9" t="s">
@@ -5898,19 +6886,40 @@
         <v>91</v>
       </c>
       <c r="AG46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AH46" s="9" t="s">
         <v>91</v>
       </c>
       <c r="AI46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AJ46" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK46" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL46" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM46" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN46" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO46" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP46" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ46" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="47" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>45</v>
       </c>
@@ -5950,7 +6959,7 @@
       <c r="M47" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N47" s="9" t="s">
+      <c r="N47" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O47" s="9" t="s">
@@ -6019,9 +7028,30 @@
       <c r="AJ47" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK47" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL47" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM47" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN47" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO47" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP47" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ47" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="48" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -6034,22 +7064,22 @@
         <v>91</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>91</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>91</v>
@@ -6060,7 +7090,7 @@
       <c r="M48" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N48" s="9" t="s">
+      <c r="N48" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O48" s="9" t="s">
@@ -6076,7 +7106,7 @@
         <v>91</v>
       </c>
       <c r="S48" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T48" s="9" t="s">
         <v>91</v>
@@ -6129,9 +7159,30 @@
       <c r="AJ48" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK48" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ48" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="49" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+    <row r="49" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -6147,7 +7198,7 @@
         <v>91</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>91</v>
@@ -6156,7 +7207,7 @@
         <v>91</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>91</v>
@@ -6170,11 +7221,11 @@
       <c r="M49" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N49" s="9" t="s">
+      <c r="N49" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O49" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P49" s="9" t="s">
         <v>91</v>
@@ -6189,7 +7240,7 @@
         <v>91</v>
       </c>
       <c r="T49" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U49" s="9" t="s">
         <v>91</v>
@@ -6239,8 +7290,29 @@
       <c r="AJ49" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK49" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL49" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM49" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN49" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO49" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP49" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ49" s="27" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="50" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>48</v>
       </c>
@@ -6280,7 +7352,7 @@
       <c r="M50" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N50" s="9" t="s">
+      <c r="N50" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O50" s="9" t="s">
@@ -6349,8 +7421,29 @@
       <c r="AJ50" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ50" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="51" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>49</v>
       </c>
@@ -6390,7 +7483,7 @@
       <c r="M51" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N51" s="9" t="s">
+      <c r="N51" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O51" s="9" t="s">
@@ -6459,8 +7552,29 @@
       <c r="AJ51" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK51" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL51" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM51" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN51" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO51" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP51" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ51" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="52" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
@@ -6500,7 +7614,7 @@
       <c r="M52" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N52" s="9" t="s">
+      <c r="N52" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O52" s="9" t="s">
@@ -6569,8 +7683,29 @@
       <c r="AJ52" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK52" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL52" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM52" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN52" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO52" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP52" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ52" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="53" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>52</v>
       </c>
@@ -6610,7 +7745,7 @@
       <c r="M53" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N53" s="9" t="s">
+      <c r="N53" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O53" s="9" t="s">
@@ -6679,8 +7814,29 @@
       <c r="AJ53" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK53" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL53" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM53" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN53" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO53" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP53" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ53" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="54" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>51</v>
       </c>
@@ -6720,7 +7876,7 @@
       <c r="M54" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N54" s="9" t="s">
+      <c r="N54" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O54" s="9" t="s">
@@ -6789,8 +7945,29 @@
       <c r="AJ54" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK54" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL54" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM54" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN54" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO54" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP54" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ54" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="55" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>53</v>
       </c>
@@ -6830,7 +8007,7 @@
       <c r="M55" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N55" s="9" t="s">
+      <c r="N55" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O55" s="9" t="s">
@@ -6899,8 +8076,29 @@
       <c r="AJ55" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK55" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL55" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM55" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN55" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO55" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP55" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ55" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="56" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>54</v>
       </c>
@@ -6940,7 +8138,7 @@
       <c r="M56" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N56" s="9" t="s">
+      <c r="N56" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O56" s="9" t="s">
@@ -7009,8 +8207,29 @@
       <c r="AJ56" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK56" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL56" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM56" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN56" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO56" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP56" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ56" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="57" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -7050,7 +8269,7 @@
       <c r="M57" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N57" s="9" t="s">
+      <c r="N57" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O57" s="9" t="s">
@@ -7119,8 +8338,29 @@
       <c r="AJ57" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK57" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL57" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM57" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN57" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO57" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP57" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ57" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="58" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>56</v>
       </c>
@@ -7160,7 +8400,7 @@
       <c r="M58" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N58" s="9" t="s">
+      <c r="N58" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O58" s="9" t="s">
@@ -7229,8 +8469,29 @@
       <c r="AJ58" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK58" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL58" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM58" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN58" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO58" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP58" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ58" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="59" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>57</v>
       </c>
@@ -7270,7 +8531,7 @@
       <c r="M59" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N59" s="9" t="s">
+      <c r="N59" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O59" s="9" t="s">
@@ -7339,8 +8600,29 @@
       <c r="AJ59" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK59" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL59" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM59" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN59" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO59" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP59" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ59" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="60" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>58</v>
       </c>
@@ -7380,7 +8662,7 @@
       <c r="M60" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N60" s="9" t="s">
+      <c r="N60" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O60" s="9" t="s">
@@ -7449,8 +8731,29 @@
       <c r="AJ60" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK60" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL60" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM60" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN60" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO60" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP60" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ60" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="61" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>59</v>
       </c>
@@ -7490,7 +8793,7 @@
       <c r="M61" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N61" s="9" t="s">
+      <c r="N61" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O61" s="9" t="s">
@@ -7559,8 +8862,29 @@
       <c r="AJ61" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK61" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL61" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM61" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN61" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO61" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP61" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ61" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="62" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>60</v>
       </c>
@@ -7600,7 +8924,7 @@
       <c r="M62" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N62" s="9" t="s">
+      <c r="N62" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O62" s="9" t="s">
@@ -7669,8 +8993,29 @@
       <c r="AJ62" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK62" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL62" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM62" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN62" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO62" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP62" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ62" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="63" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>61</v>
       </c>
@@ -7710,7 +9055,7 @@
       <c r="M63" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N63" s="9" t="s">
+      <c r="N63" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O63" s="9" t="s">
@@ -7779,8 +9124,29 @@
       <c r="AJ63" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK63" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL63" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM63" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN63" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO63" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP63" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ63" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="64" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>62</v>
       </c>
@@ -7820,7 +9186,7 @@
       <c r="M64" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N64" s="9" t="s">
+      <c r="N64" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O64" s="9" t="s">
@@ -7889,8 +9255,29 @@
       <c r="AJ64" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="AK64" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL64" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM64" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN64" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO64" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP64" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ64" s="27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="65" spans="1:36" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:43" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>63</v>
       </c>
@@ -7930,7 +9317,7 @@
       <c r="M65" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N65" s="9" t="s">
+      <c r="N65" s="32" t="s">
         <v>91</v>
       </c>
       <c r="O65" s="9" t="s">
@@ -7997,6 +9384,27 @@
         <v>91</v>
       </c>
       <c r="AJ65" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK65" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL65" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM65" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN65" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO65" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP65" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ65" s="27" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Buncha stuff lab 4
</commit_message>
<xml_diff>
--- a/Lab 4/control_store_lab_4.xlsx
+++ b/Lab 4/control_store_lab_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffacd89b2f1a651/Documents/Current Classes/ECE 460N/Labs/Lab 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1463" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35DC26AC-B2CB-4779-873B-B9DEE093F9A1}"/>
+  <xr:revisionPtr revIDLastSave="1509" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A73A48F4-E12E-4E0A-A97A-FBA4011D877C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Store" sheetId="1" r:id="rId1"/>
@@ -298,12 +298,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>LD.TEMP</t>
-  </si>
-  <si>
-    <t>GATETEMP</t>
-  </si>
-  <si>
     <t>LD.PRIV</t>
   </si>
   <si>
@@ -347,6 +341,12 @@
   </si>
   <si>
     <t xml:space="preserve"> EXCVMUX</t>
+  </si>
+  <si>
+    <t>LD.INT_EN</t>
+  </si>
+  <si>
+    <t>INT_ENMUX</t>
   </si>
 </sst>
 </file>
@@ -614,13 +614,13 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,9 +937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BC55" sqref="BC55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -953,8 +953,9 @@
     <col min="16" max="16" width="2.453125" style="32" customWidth="1"/>
     <col min="17" max="17" width="2.453125" style="6" customWidth="1"/>
     <col min="18" max="40" width="2.453125" style="1" customWidth="1"/>
-    <col min="41" max="56" width="2.453125" style="3" customWidth="1"/>
-    <col min="57" max="58" width="2.453125" style="1" customWidth="1"/>
+    <col min="41" max="54" width="2.453125" style="3" customWidth="1"/>
+    <col min="55" max="56" width="2.453125" style="1" customWidth="1"/>
+    <col min="57" max="58" width="2.453125" style="3" customWidth="1"/>
     <col min="59" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
@@ -964,21 +965,21 @@
         <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
       <c r="M1" s="2" t="s">
         <v>67</v>
       </c>
@@ -1015,32 +1016,32 @@
       <c r="X1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" s="37" t="s">
+      <c r="Y1" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37" t="s">
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="36" t="s">
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="36"/>
+      <c r="AD1" s="37"/>
       <c r="AE1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="37" t="s">
+      <c r="AF1" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" s="37"/>
+      <c r="AG1" s="38"/>
       <c r="AH1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="37" t="s">
+      <c r="AI1" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" s="37"/>
+      <c r="AJ1" s="38"/>
       <c r="AK1" s="2" t="s">
         <v>86</v>
       </c>
@@ -1054,10 +1055,10 @@
         <v>89</v>
       </c>
       <c r="AO1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP1" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="AQ1" s="2" t="s">
         <v>94</v>
@@ -1071,16 +1072,16 @@
       <c r="AT1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AU1" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AW1" s="36" t="s">
+      <c r="AX1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AX1" s="36"/>
       <c r="AY1" s="2" t="s">
         <v>101</v>
       </c>
@@ -1091,18 +1092,18 @@
         <v>103</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="BC1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BC1" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="BD1" s="37"/>
+      <c r="BE1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="BE1" s="36" t="s">
+      <c r="BF1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="BF1" s="36"/>
     </row>
     <row r="2" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
@@ -1243,16 +1244,16 @@
       <c r="AT2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW2" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX2" s="17" t="s">
+      <c r="AU2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX2" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY2" s="26" t="s">
@@ -1267,16 +1268,16 @@
       <c r="BB2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE2" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF2" s="17" t="s">
+      <c r="BC2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF2" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1419,16 +1420,16 @@
       <c r="AT3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU3" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV3" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW3" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX3" s="17" t="s">
+      <c r="AU3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW3" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX3" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY3" s="26" t="s">
@@ -1443,16 +1444,16 @@
       <c r="BB3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC3" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD3" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE3" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF3" s="17" t="s">
+      <c r="BC3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE3" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF3" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1595,16 +1596,16 @@
       <c r="AT4" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW4" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX4" s="17" t="s">
+      <c r="AU4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW4" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX4" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY4" s="26" t="s">
@@ -1619,16 +1620,16 @@
       <c r="BB4" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE4" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF4" s="17" t="s">
+      <c r="BC4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE4" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF4" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1771,16 +1772,16 @@
       <c r="AT5" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU5" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV5" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW5" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX5" s="17" t="s">
+      <c r="AU5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV5" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW5" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX5" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY5" s="26" t="s">
@@ -1795,16 +1796,16 @@
       <c r="BB5" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC5" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD5" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE5" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF5" s="17" t="s">
+      <c r="BC5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD5" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE5" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF5" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1947,16 +1948,16 @@
       <c r="AT6" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX6" s="17" t="s">
+      <c r="AU6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV6" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW6" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX6" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY6" s="26" t="s">
@@ -1971,16 +1972,16 @@
       <c r="BB6" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF6" s="17" t="s">
+      <c r="BC6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD6" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE6" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF6" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2123,16 +2124,16 @@
       <c r="AT7" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU7" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV7" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW7" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX7" s="17" t="s">
+      <c r="AU7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV7" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW7" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX7" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY7" s="26" t="s">
@@ -2147,16 +2148,16 @@
       <c r="BB7" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC7" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD7" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE7" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF7" s="17" t="s">
+      <c r="BC7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD7" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE7" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF7" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2299,16 +2300,16 @@
       <c r="AT8" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU8" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV8" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW8" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX8" s="17" t="s">
+      <c r="AU8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV8" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW8" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX8" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY8" s="26" t="s">
@@ -2323,16 +2324,16 @@
       <c r="BB8" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC8" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD8" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE8" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF8" s="17" t="s">
+      <c r="BC8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD8" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE8" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF8" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2475,16 +2476,16 @@
       <c r="AT9" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU9" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV9" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW9" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX9" s="17" t="s">
+      <c r="AU9" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV9" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW9" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX9" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY9" s="26" t="s">
@@ -2499,16 +2500,16 @@
       <c r="BB9" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC9" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD9" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE9" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF9" s="17" t="s">
+      <c r="BC9" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD9" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE9" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF9" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2651,16 +2652,16 @@
       <c r="AT10" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU10" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV10" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW10" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX10" s="17" t="s">
+      <c r="AU10" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW10" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX10" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY10" s="26" t="s">
@@ -2675,16 +2676,16 @@
       <c r="BB10" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC10" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD10" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE10" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF10" s="17" t="s">
+      <c r="BC10" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE10" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF10" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2827,16 +2828,16 @@
       <c r="AT11" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU11" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV11" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW11" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX11" s="17" t="s">
+      <c r="AU11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX11" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY11" s="26" t="s">
@@ -2851,16 +2852,16 @@
       <c r="BB11" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC11" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD11" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE11" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF11" s="17" t="s">
+      <c r="BC11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF11" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3003,16 +3004,16 @@
       <c r="AT12" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU12" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV12" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW12" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX12" s="17" t="s">
+      <c r="AU12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV12" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW12" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX12" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY12" s="26" t="s">
@@ -3025,18 +3026,18 @@
         <v>91</v>
       </c>
       <c r="BB12" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC12" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD12" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BE12" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="BF12" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC12" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="BD12" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE12" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF12" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3179,16 +3180,16 @@
       <c r="AT13" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU13" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV13" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW13" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX13" s="17" t="s">
+      <c r="AU13" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV13" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX13" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY13" s="26" t="s">
@@ -3201,18 +3202,18 @@
         <v>91</v>
       </c>
       <c r="BB13" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC13" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD13" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BE13" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="BF13" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC13" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="BD13" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF13" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3355,16 +3356,16 @@
       <c r="AT14" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU14" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV14" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW14" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX14" s="17" t="s">
+      <c r="AU14" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV14" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX14" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY14" s="26" t="s">
@@ -3379,16 +3380,16 @@
       <c r="BB14" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC14" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD14" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE14" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF14" s="17" t="s">
+      <c r="BC14" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD14" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF14" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3531,16 +3532,16 @@
       <c r="AT15" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU15" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV15" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW15" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX15" s="17" t="s">
+      <c r="AU15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW15" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX15" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY15" s="26" t="s">
@@ -3555,16 +3556,16 @@
       <c r="BB15" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC15" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD15" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE15" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF15" s="17" t="s">
+      <c r="BC15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE15" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF15" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3707,16 +3708,16 @@
       <c r="AT16" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU16" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV16" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW16" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX16" s="17" t="s">
+      <c r="AU16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV16" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW16" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX16" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY16" s="26" t="s">
@@ -3731,16 +3732,16 @@
       <c r="BB16" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC16" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD16" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE16" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF16" s="17" t="s">
+      <c r="BC16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD16" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE16" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF16" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3883,16 +3884,16 @@
       <c r="AT17" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW17" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX17" s="17" t="s">
+      <c r="AU17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV17" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW17" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX17" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY17" s="26" t="s">
@@ -3907,16 +3908,16 @@
       <c r="BB17" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE17" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF17" s="17" t="s">
+      <c r="BC17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD17" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE17" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF17" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4059,16 +4060,16 @@
       <c r="AT18" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU18" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV18" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW18" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX18" s="17" t="s">
+      <c r="AU18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV18" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW18" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX18" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY18" s="26" t="s">
@@ -4083,16 +4084,16 @@
       <c r="BB18" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC18" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD18" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE18" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF18" s="17" t="s">
+      <c r="BC18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD18" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE18" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF18" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4235,16 +4236,16 @@
       <c r="AT19" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU19" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV19" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW19" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX19" s="17" t="s">
+      <c r="AU19" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV19" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW19" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX19" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY19" s="26" t="s">
@@ -4259,16 +4260,16 @@
       <c r="BB19" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC19" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD19" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE19" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF19" s="17" t="s">
+      <c r="BC19" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD19" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE19" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF19" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4411,16 +4412,16 @@
       <c r="AT20" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU20" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV20" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW20" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX20" s="17" t="s">
+      <c r="AU20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV20" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW20" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX20" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY20" s="26" t="s">
@@ -4435,16 +4436,16 @@
       <c r="BB20" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC20" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD20" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE20" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF20" s="17" t="s">
+      <c r="BC20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD20" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE20" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF20" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4587,16 +4588,16 @@
       <c r="AT21" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU21" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV21" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW21" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX21" s="17" t="s">
+      <c r="AU21" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV21" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW21" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX21" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY21" s="26" t="s">
@@ -4611,16 +4612,16 @@
       <c r="BB21" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC21" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD21" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE21" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF21" s="17" t="s">
+      <c r="BC21" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD21" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE21" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF21" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4763,16 +4764,16 @@
       <c r="AT22" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU22" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV22" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW22" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX22" s="17" t="s">
+      <c r="AU22" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV22" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW22" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX22" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY22" s="26" t="s">
@@ -4787,16 +4788,16 @@
       <c r="BB22" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC22" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD22" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE22" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF22" s="17" t="s">
+      <c r="BC22" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD22" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE22" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF22" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4939,16 +4940,16 @@
       <c r="AT23" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW23" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX23" s="17" t="s">
+      <c r="AU23" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV23" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW23" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX23" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY23" s="26" t="s">
@@ -4963,16 +4964,16 @@
       <c r="BB23" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE23" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF23" s="17" t="s">
+      <c r="BC23" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD23" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE23" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF23" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -5115,16 +5116,16 @@
       <c r="AT24" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU24" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV24" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW24" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX24" s="17" t="s">
+      <c r="AU24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW24" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX24" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY24" s="26" t="s">
@@ -5139,16 +5140,16 @@
       <c r="BB24" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC24" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD24" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE24" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF24" s="17" t="s">
+      <c r="BC24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE24" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF24" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -5291,16 +5292,16 @@
       <c r="AT25" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU25" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV25" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW25" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX25" s="17" t="s">
+      <c r="AU25" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV25" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW25" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX25" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY25" s="26" t="s">
@@ -5315,16 +5316,16 @@
       <c r="BB25" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC25" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD25" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE25" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF25" s="17" t="s">
+      <c r="BC25" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD25" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE25" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF25" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -5467,16 +5468,16 @@
       <c r="AT26" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU26" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV26" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW26" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX26" s="17" t="s">
+      <c r="AU26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV26" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW26" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX26" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY26" s="26" t="s">
@@ -5491,16 +5492,16 @@
       <c r="BB26" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC26" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD26" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE26" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF26" s="17" t="s">
+      <c r="BC26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD26" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE26" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF26" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -5643,16 +5644,16 @@
       <c r="AT27" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU27" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV27" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW27" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX27" s="17" t="s">
+      <c r="AU27" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV27" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW27" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX27" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY27" s="26" t="s">
@@ -5667,21 +5668,21 @@
       <c r="BB27" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC27" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD27" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE27" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF27" s="17" t="s">
+      <c r="BC27" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD27" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE27" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF27" s="26" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="36" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -5691,168 +5692,168 @@
         <v>91</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>90</v>
+      <c r="G28" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>90</v>
+      <c r="K28" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="M28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="M28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="N28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="O28" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="P28" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q28" s="13" t="s">
+      <c r="O28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="R28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="S28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="S28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="T28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="U28" s="13" t="s">
+      <c r="U28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="V28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="W28" s="13" t="s">
+      <c r="W28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="X28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="Y28" s="13" t="s">
+      <c r="Y28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="Z28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AA28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB28" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD28" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE28" s="13" t="s">
+      <c r="AA28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="AF28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AG28" s="13" t="s">
+      <c r="AG28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="AH28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AI28" s="13" t="s">
+      <c r="AI28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="AJ28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AK28" s="13" t="s">
+      <c r="AK28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="AL28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AM28" s="13" t="s">
+      <c r="AM28" s="14" t="s">
         <v>91</v>
       </c>
       <c r="AN28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AO28" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ28" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AR28" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS28" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AU28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX28" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AZ28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BA28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BB28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF28" s="17" t="s">
+      <c r="AO28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BA28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BB28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BC28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE28" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF28" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -5995,16 +5996,16 @@
       <c r="AT29" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU29" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV29" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX29" s="17" t="s">
+      <c r="AU29" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV29" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW29" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX29" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY29" s="26" t="s">
@@ -6019,16 +6020,16 @@
       <c r="BB29" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC29" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD29" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF29" s="17" t="s">
+      <c r="BC29" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD29" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE29" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF29" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6171,16 +6172,16 @@
       <c r="AT30" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU30" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV30" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW30" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX30" s="17" t="s">
+      <c r="AU30" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV30" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW30" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX30" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY30" s="26" t="s">
@@ -6195,16 +6196,16 @@
       <c r="BB30" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC30" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD30" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE30" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF30" s="17" t="s">
+      <c r="BC30" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD30" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE30" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF30" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6347,16 +6348,16 @@
       <c r="AT31" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU31" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV31" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW31" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX31" s="17" t="s">
+      <c r="AU31" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV31" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW31" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX31" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY31" s="26" t="s">
@@ -6371,16 +6372,16 @@
       <c r="BB31" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC31" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD31" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE31" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF31" s="17" t="s">
+      <c r="BC31" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD31" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE31" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF31" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6523,16 +6524,16 @@
       <c r="AT32" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU32" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV32" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW32" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX32" s="17" t="s">
+      <c r="AU32" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV32" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW32" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX32" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY32" s="26" t="s">
@@ -6547,16 +6548,16 @@
       <c r="BB32" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC32" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD32" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE32" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF32" s="17" t="s">
+      <c r="BC32" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD32" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE32" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF32" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6699,16 +6700,16 @@
       <c r="AT33" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU33" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV33" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW33" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX33" s="17" t="s">
+      <c r="AU33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV33" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW33" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX33" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY33" s="26" t="s">
@@ -6723,16 +6724,16 @@
       <c r="BB33" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC33" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD33" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE33" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF33" s="17" t="s">
+      <c r="BC33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD33" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE33" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF33" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6875,16 +6876,16 @@
       <c r="AT34" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU34" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV34" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW34" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX34" s="17" t="s">
+      <c r="AU34" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV34" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW34" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX34" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY34" s="26" t="s">
@@ -6899,16 +6900,16 @@
       <c r="BB34" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC34" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD34" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE34" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF34" s="17" t="s">
+      <c r="BC34" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD34" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE34" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF34" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -7051,16 +7052,16 @@
       <c r="AT35" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU35" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV35" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW35" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX35" s="17" t="s">
+      <c r="AU35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV35" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW35" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX35" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY35" s="26" t="s">
@@ -7075,16 +7076,16 @@
       <c r="BB35" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC35" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD35" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE35" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF35" s="17" t="s">
+      <c r="BC35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD35" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE35" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF35" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -7227,20 +7228,20 @@
       <c r="AT36" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="AU36" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV36" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW36" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX36" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY36" s="34" t="s">
-        <v>90</v>
+      <c r="AU36" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV36" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW36" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX36" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY36" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="AZ36" s="26" t="s">
         <v>91</v>
@@ -7251,16 +7252,16 @@
       <c r="BB36" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC36" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD36" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE36" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF36" s="17" t="s">
+      <c r="BC36" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD36" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE36" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF36" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -7403,16 +7404,16 @@
       <c r="AT37" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU37" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV37" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW37" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX37" s="17" t="s">
+      <c r="AU37" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV37" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW37" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX37" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY37" s="26" t="s">
@@ -7427,16 +7428,16 @@
       <c r="BB37" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC37" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD37" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE37" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF37" s="17" t="s">
+      <c r="BC37" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD37" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE37" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF37" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -7579,16 +7580,16 @@
       <c r="AT38" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU38" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV38" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW38" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX38" s="17" t="s">
+      <c r="AU38" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV38" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW38" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX38" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY38" s="26" t="s">
@@ -7603,16 +7604,16 @@
       <c r="BB38" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC38" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD38" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE38" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF38" s="17" t="s">
+      <c r="BC38" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD38" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE38" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF38" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -7755,16 +7756,16 @@
       <c r="AT39" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU39" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV39" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW39" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX39" s="17" t="s">
+      <c r="AU39" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV39" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW39" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX39" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY39" s="26" t="s">
@@ -7779,16 +7780,16 @@
       <c r="BB39" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC39" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD39" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE39" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF39" s="17" t="s">
+      <c r="BC39" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD39" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE39" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF39" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -7931,16 +7932,16 @@
       <c r="AT40" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU40" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV40" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW40" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX40" s="17" t="s">
+      <c r="AU40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV40" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW40" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX40" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY40" s="26" t="s">
@@ -7955,16 +7956,16 @@
       <c r="BB40" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC40" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD40" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE40" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF40" s="17" t="s">
+      <c r="BC40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD40" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE40" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF40" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8021,7 +8022,7 @@
         <v>91</v>
       </c>
       <c r="R41" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S41" s="9" t="s">
         <v>91</v>
@@ -8090,13 +8091,13 @@
         <v>91</v>
       </c>
       <c r="AO41" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AP41" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AQ41" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AR41" s="26" t="s">
         <v>91</v>
@@ -8107,16 +8108,16 @@
       <c r="AT41" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU41" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV41" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW41" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX41" s="17" t="s">
+      <c r="AU41" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV41" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW41" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX41" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY41" s="26" t="s">
@@ -8131,16 +8132,16 @@
       <c r="BB41" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC41" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD41" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE41" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF41" s="17" t="s">
+      <c r="BC41" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD41" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE41" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF41" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8155,31 +8156,31 @@
         <v>91</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="G42" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="H42" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="I42" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="K42" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="L42" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L42" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="M42" s="31" t="s">
         <v>91</v>
@@ -8283,20 +8284,20 @@
       <c r="AT42" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="AU42" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV42" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW42" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX42" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY42" s="34" t="s">
-        <v>90</v>
+      <c r="AU42" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV42" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW42" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX42" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY42" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="AZ42" s="26" t="s">
         <v>91</v>
@@ -8307,16 +8308,16 @@
       <c r="BB42" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC42" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD42" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE42" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF42" s="17" t="s">
+      <c r="BC42" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD42" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE42" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BF42" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8459,16 +8460,16 @@
       <c r="AT43" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU43" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV43" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW43" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX43" s="17" t="s">
+      <c r="AU43" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV43" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW43" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX43" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY43" s="26" t="s">
@@ -8483,21 +8484,21 @@
       <c r="BB43" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC43" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD43" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE43" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF43" s="17" t="s">
+      <c r="BC43" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD43" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE43" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF43" s="26" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -8662,13 +8663,13 @@
       <c r="BC44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="BD44" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE44" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF44" s="17" t="s">
+      <c r="BD44" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE44" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF44" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8811,23 +8812,23 @@
       <c r="AT45" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU45" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV45" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW45" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX45" s="17" t="s">
-        <v>91</v>
+      <c r="AU45" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV45" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW45" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX45" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="AY45" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AZ45" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BA45" s="26" t="s">
         <v>91</v>
@@ -8835,16 +8836,16 @@
       <c r="BB45" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC45" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD45" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE45" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF45" s="17" t="s">
+      <c r="BC45" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD45" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE45" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF45" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8987,16 +8988,16 @@
       <c r="AT46" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU46" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV46" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW46" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX46" s="17" t="s">
+      <c r="AU46" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV46" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW46" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX46" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY46" s="26" t="s">
@@ -9011,16 +9012,16 @@
       <c r="BB46" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC46" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD46" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE46" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF46" s="17" t="s">
+      <c r="BC46" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD46" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE46" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF46" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -9163,20 +9164,20 @@
       <c r="AT47" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU47" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV47" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW47" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX47" s="17" t="s">
-        <v>90</v>
+      <c r="AU47" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV47" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW47" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX47" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="AY47" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AZ47" s="26" t="s">
         <v>91</v>
@@ -9187,16 +9188,16 @@
       <c r="BB47" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC47" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD47" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE47" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF47" s="17" t="s">
+      <c r="BC47" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD47" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE47" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF47" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -9339,40 +9340,40 @@
       <c r="AT48" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU48" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV48" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW48" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX48" s="17" t="s">
+      <c r="AU48" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV48" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW48" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX48" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY48" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AZ48" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="BA48" s="26" t="s">
         <v>91</v>
       </c>
       <c r="BB48" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BC48" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD48" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE48" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF48" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BC48" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD48" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE48" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF48" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -9515,16 +9516,16 @@
       <c r="AT49" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU49" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV49" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW49" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX49" s="17" t="s">
+      <c r="AU49" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV49" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW49" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX49" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY49" s="26" t="s">
@@ -9537,18 +9538,18 @@
         <v>91</v>
       </c>
       <c r="BB49" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC49" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD49" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BE49" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF49" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC49" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD49" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE49" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF49" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -9691,16 +9692,16 @@
       <c r="AT50" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU50" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV50" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW50" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX50" s="17" t="s">
+      <c r="AU50" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV50" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW50" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX50" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY50" s="26" t="s">
@@ -9713,19 +9714,19 @@
         <v>91</v>
       </c>
       <c r="BB50" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC50" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD50" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BE50" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF50" s="17" t="s">
-        <v>90</v>
+        <v>90</v>
+      </c>
+      <c r="BC50" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD50" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="BE50" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF50" s="26" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
@@ -9850,62 +9851,62 @@
         <v>91</v>
       </c>
       <c r="AO51" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AP51" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AQ51" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AR51" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AS51" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AT51" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU51" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV51" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW51" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX51" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU51" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV51" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW51" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX51" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY51" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AZ51" s="26" t="s">
         <v>91</v>
       </c>
       <c r="BA51" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BB51" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC51" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD51" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE51" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF51" s="17" t="s">
+      <c r="BC51" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD51" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE51" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF51" s="26" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="36" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="9" t="s">
@@ -10073,10 +10074,10 @@
       <c r="BD52" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BE52" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF52" s="9" t="s">
+      <c r="BE52" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF52" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -10219,16 +10220,16 @@
       <c r="AT53" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU53" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV53" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW53" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX53" s="17" t="s">
+      <c r="AU53" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV53" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW53" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX53" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY53" s="26" t="s">
@@ -10243,16 +10244,16 @@
       <c r="BB53" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC53" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD53" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE53" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF53" s="17" t="s">
+      <c r="BC53" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD53" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE53" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF53" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -10395,16 +10396,16 @@
       <c r="AT54" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU54" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV54" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW54" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX54" s="17" t="s">
+      <c r="AU54" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV54" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW54" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX54" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY54" s="26" t="s">
@@ -10419,16 +10420,16 @@
       <c r="BB54" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC54" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD54" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE54" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF54" s="17" t="s">
+      <c r="BC54" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD54" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE54" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF54" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -10455,19 +10456,19 @@
         <v>90</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>90</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M55" s="9" t="s">
         <v>91</v>
@@ -10554,37 +10555,37 @@
         <v>91</v>
       </c>
       <c r="AO55" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AP55" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AQ55" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AR55" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AS55" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AT55" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU55" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV55" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW55" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX55" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU55" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV55" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW55" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX55" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY55" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AZ55" s="26" t="s">
         <v>91</v>
@@ -10595,17 +10596,17 @@
       <c r="BB55" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC55" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BD55" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE55" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF55" s="17" t="s">
-        <v>91</v>
+      <c r="BC55" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD55" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE55" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BF55" s="26" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
@@ -10747,16 +10748,16 @@
       <c r="AT56" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU56" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV56" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW56" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX56" s="17" t="s">
+      <c r="AU56" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV56" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW56" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX56" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY56" s="26" t="s">
@@ -10771,16 +10772,16 @@
       <c r="BB56" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC56" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD56" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE56" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF56" s="17" t="s">
+      <c r="BC56" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD56" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE56" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF56" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -10923,20 +10924,20 @@
       <c r="AT57" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU57" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV57" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW57" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX57" s="17" t="s">
-        <v>90</v>
+      <c r="AU57" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV57" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW57" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX57" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="AY57" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AZ57" s="26" t="s">
         <v>91</v>
@@ -10947,16 +10948,16 @@
       <c r="BB57" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC57" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD57" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE57" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF57" s="17" t="s">
+      <c r="BC57" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD57" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE57" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF57" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11099,16 +11100,16 @@
       <c r="AT58" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU58" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV58" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW58" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX58" s="17" t="s">
+      <c r="AU58" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV58" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW58" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX58" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY58" s="26" t="s">
@@ -11123,16 +11124,16 @@
       <c r="BB58" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC58" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD58" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE58" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF58" s="17" t="s">
+      <c r="BC58" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD58" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE58" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF58" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11275,16 +11276,16 @@
       <c r="AT59" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU59" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV59" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW59" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX59" s="17" t="s">
+      <c r="AU59" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV59" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW59" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX59" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY59" s="26" t="s">
@@ -11299,16 +11300,16 @@
       <c r="BB59" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC59" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD59" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE59" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF59" s="17" t="s">
+      <c r="BC59" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD59" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE59" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF59" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11451,16 +11452,16 @@
       <c r="AT60" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU60" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV60" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW60" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX60" s="17" t="s">
+      <c r="AU60" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV60" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW60" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX60" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY60" s="26" t="s">
@@ -11475,16 +11476,16 @@
       <c r="BB60" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC60" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD60" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE60" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF60" s="17" t="s">
+      <c r="BC60" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD60" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE60" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF60" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11622,25 +11623,25 @@
         <v>91</v>
       </c>
       <c r="AS61" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AT61" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU61" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV61" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW61" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AX61" s="17" t="s">
-        <v>90</v>
+      <c r="AU61" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV61" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW61" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX61" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="AY61" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AZ61" s="26" t="s">
         <v>91</v>
@@ -11651,16 +11652,16 @@
       <c r="BB61" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC61" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD61" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE61" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF61" s="17" t="s">
+      <c r="BC61" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD61" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE61" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF61" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11803,16 +11804,16 @@
       <c r="AT62" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU62" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV62" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW62" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX62" s="17" t="s">
+      <c r="AU62" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV62" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW62" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX62" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY62" s="26" t="s">
@@ -11827,16 +11828,16 @@
       <c r="BB62" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC62" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD62" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE62" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF62" s="17" t="s">
+      <c r="BC62" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD62" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE62" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF62" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11979,16 +11980,16 @@
       <c r="AT63" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU63" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV63" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW63" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX63" s="17" t="s">
+      <c r="AU63" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV63" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW63" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX63" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY63" s="26" t="s">
@@ -12003,16 +12004,16 @@
       <c r="BB63" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC63" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD63" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE63" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF63" s="17" t="s">
+      <c r="BC63" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD63" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE63" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF63" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12155,16 +12156,16 @@
       <c r="AT64" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AU64" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV64" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW64" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX64" s="17" t="s">
+      <c r="AU64" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV64" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW64" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX64" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY64" s="26" t="s">
@@ -12179,16 +12180,16 @@
       <c r="BB64" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC64" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD64" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE64" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF64" s="17" t="s">
+      <c r="BC64" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD64" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE64" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF64" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12329,22 +12330,22 @@
         <v>91</v>
       </c>
       <c r="AT65" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AU65" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV65" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW65" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AX65" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU65" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV65" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW65" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX65" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AY65" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AZ65" s="26" t="s">
         <v>91</v>
@@ -12355,23 +12356,23 @@
       <c r="BB65" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BC65" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD65" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE65" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF65" s="17" t="s">
+      <c r="BC65" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD65" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE65" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF65" s="26" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="BE1:BF1"/>
-    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="AU1:AV1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="AI1:AJ1"/>
     <mergeCell ref="G1:L1"/>

</xml_diff>

<commit_message>
Remove Interrupt Enable Bit
</commit_message>
<xml_diff>
--- a/Lab 4/control_store_lab_4.xlsx
+++ b/Lab 4/control_store_lab_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffacd89b2f1a651/Documents/Current Classes/ECE 460N/Labs/Lab 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1515" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75E8B3AD-A383-4506-9C61-46EB8349DEBD}"/>
+  <xr:revisionPtr revIDLastSave="1523" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF54CB4C-C67D-4E8B-9C3C-AAE77AFD02AB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3755" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3625" uniqueCount="107">
   <si>
     <t>000000  (state 0)</t>
   </si>
@@ -340,13 +340,7 @@
     <t>LD.EXCV</t>
   </si>
   <si>
-    <t xml:space="preserve"> EXCVMUX</t>
-  </si>
-  <si>
-    <t>LD.INT_EN</t>
-  </si>
-  <si>
-    <t>INT_ENMUX</t>
+    <t xml:space="preserve"> EXCVectMUX</t>
   </si>
 </sst>
 </file>
@@ -543,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -615,6 +609,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -937,9 +934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL8" sqref="AL8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BG5" sqref="BG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -967,19 +964,19 @@
       <c r="C1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
       <c r="M1" s="2" t="s">
         <v>67</v>
       </c>
@@ -1016,32 +1013,32 @@
       <c r="X1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="Y1" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38" t="s">
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="37" t="s">
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="37"/>
+      <c r="AD1" s="38"/>
       <c r="AE1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="38" t="s">
+      <c r="AF1" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" s="38"/>
+      <c r="AG1" s="39"/>
       <c r="AH1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="38" t="s">
+      <c r="AI1" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" s="38"/>
+      <c r="AJ1" s="39"/>
       <c r="AK1" s="2" t="s">
         <v>86</v>
       </c>
@@ -1054,56 +1051,52 @@
       <c r="AN1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="27" t="s">
         <v>97</v>
       </c>
       <c r="AU1" s="37" t="s">
         <v>98</v>
       </c>
       <c r="AV1" s="37"/>
-      <c r="AW1" s="2" t="s">
+      <c r="AW1" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AX1" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AY1" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AZ1" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BA1" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="27" t="s">
         <v>105</v>
       </c>
       <c r="BC1" s="37" t="s">
         <v>106</v>
       </c>
       <c r="BD1" s="37"/>
-      <c r="BE1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BF1" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="BE1" s="27"/>
+      <c r="BF1" s="27"/>
     </row>
     <row r="2" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
@@ -1274,12 +1267,8 @@
       <c r="BD2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF2" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE2" s="26"/>
+      <c r="BF2" s="26"/>
     </row>
     <row r="3" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
@@ -1450,12 +1439,8 @@
       <c r="BD3" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE3" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF3" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE3" s="26"/>
+      <c r="BF3" s="26"/>
     </row>
     <row r="4" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
@@ -1626,12 +1611,8 @@
       <c r="BD4" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF4" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE4" s="26"/>
+      <c r="BF4" s="26"/>
     </row>
     <row r="5" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
@@ -1802,12 +1783,8 @@
       <c r="BD5" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE5" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF5" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE5" s="26"/>
+      <c r="BF5" s="26"/>
     </row>
     <row r="6" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
@@ -1978,12 +1955,8 @@
       <c r="BD6" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF6" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE6" s="26"/>
+      <c r="BF6" s="26"/>
     </row>
     <row r="7" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
@@ -2154,12 +2127,8 @@
       <c r="BD7" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE7" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF7" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE7" s="26"/>
+      <c r="BF7" s="26"/>
     </row>
     <row r="8" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
@@ -2330,12 +2299,8 @@
       <c r="BD8" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE8" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF8" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE8" s="26"/>
+      <c r="BF8" s="26"/>
     </row>
     <row r="9" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
@@ -2506,12 +2471,8 @@
       <c r="BD9" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE9" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF9" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE9" s="26"/>
+      <c r="BF9" s="26"/>
     </row>
     <row r="10" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
@@ -2682,12 +2643,8 @@
       <c r="BD10" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE10" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF10" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE10" s="26"/>
+      <c r="BF10" s="26"/>
     </row>
     <row r="11" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
@@ -2858,12 +2815,8 @@
       <c r="BD11" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE11" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF11" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE11" s="26"/>
+      <c r="BF11" s="26"/>
     </row>
     <row r="12" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
@@ -3034,12 +2987,8 @@
       <c r="BD12" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE12" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF12" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE12" s="26"/>
+      <c r="BF12" s="26"/>
     </row>
     <row r="13" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
@@ -3210,12 +3159,8 @@
       <c r="BD13" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE13" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF13" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE13" s="26"/>
+      <c r="BF13" s="26"/>
     </row>
     <row r="14" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
@@ -3386,12 +3331,8 @@
       <c r="BD14" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE14" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF14" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE14" s="26"/>
+      <c r="BF14" s="26"/>
     </row>
     <row r="15" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
@@ -3562,12 +3503,8 @@
       <c r="BD15" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE15" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF15" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE15" s="26"/>
+      <c r="BF15" s="26"/>
     </row>
     <row r="16" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
@@ -3738,12 +3675,8 @@
       <c r="BD16" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE16" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF16" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE16" s="26"/>
+      <c r="BF16" s="26"/>
     </row>
     <row r="17" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
@@ -3914,12 +3847,8 @@
       <c r="BD17" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF17" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE17" s="26"/>
+      <c r="BF17" s="26"/>
     </row>
     <row r="18" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
@@ -4090,12 +4019,8 @@
       <c r="BD18" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE18" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF18" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE18" s="26"/>
+      <c r="BF18" s="26"/>
     </row>
     <row r="19" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
@@ -4266,12 +4191,8 @@
       <c r="BD19" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE19" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF19" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE19" s="26"/>
+      <c r="BF19" s="26"/>
     </row>
     <row r="20" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
@@ -4442,12 +4363,8 @@
       <c r="BD20" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE20" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF20" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE20" s="26"/>
+      <c r="BF20" s="26"/>
     </row>
     <row r="21" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
@@ -4618,12 +4535,8 @@
       <c r="BD21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE21" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF21" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE21" s="26"/>
+      <c r="BF21" s="26"/>
     </row>
     <row r="22" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
@@ -4794,12 +4707,8 @@
       <c r="BD22" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE22" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF22" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE22" s="26"/>
+      <c r="BF22" s="26"/>
     </row>
     <row r="23" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
@@ -4970,12 +4879,8 @@
       <c r="BD23" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF23" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE23" s="26"/>
+      <c r="BF23" s="26"/>
     </row>
     <row r="24" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
@@ -5146,12 +5051,8 @@
       <c r="BD24" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE24" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF24" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE24" s="26"/>
+      <c r="BF24" s="26"/>
     </row>
     <row r="25" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
@@ -5322,12 +5223,8 @@
       <c r="BD25" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE25" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF25" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE25" s="26"/>
+      <c r="BF25" s="26"/>
     </row>
     <row r="26" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
@@ -5498,12 +5395,8 @@
       <c r="BD26" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE26" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF26" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE26" s="26"/>
+      <c r="BF26" s="26"/>
     </row>
     <row r="27" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
@@ -5674,12 +5567,8 @@
       <c r="BD27" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE27" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF27" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE27" s="26"/>
+      <c r="BF27" s="26"/>
     </row>
     <row r="28" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
@@ -5850,12 +5739,8 @@
       <c r="BD28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BE28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF28" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE28" s="26"/>
+      <c r="BF28" s="26"/>
     </row>
     <row r="29" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
@@ -6026,12 +5911,8 @@
       <c r="BD29" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE29" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF29" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE29" s="26"/>
+      <c r="BF29" s="26"/>
     </row>
     <row r="30" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
@@ -6202,12 +6083,8 @@
       <c r="BD30" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE30" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF30" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE30" s="26"/>
+      <c r="BF30" s="26"/>
     </row>
     <row r="31" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
@@ -6378,12 +6255,8 @@
       <c r="BD31" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE31" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF31" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE31" s="26"/>
+      <c r="BF31" s="26"/>
     </row>
     <row r="32" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
@@ -6554,12 +6427,8 @@
       <c r="BD32" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE32" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF32" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE32" s="26"/>
+      <c r="BF32" s="26"/>
     </row>
     <row r="33" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
@@ -6730,12 +6599,8 @@
       <c r="BD33" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE33" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF33" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE33" s="26"/>
+      <c r="BF33" s="26"/>
     </row>
     <row r="34" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
@@ -6906,12 +6771,8 @@
       <c r="BD34" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE34" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF34" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE34" s="26"/>
+      <c r="BF34" s="26"/>
     </row>
     <row r="35" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
@@ -7082,12 +6943,8 @@
       <c r="BD35" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE35" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF35" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE35" s="26"/>
+      <c r="BF35" s="26"/>
     </row>
     <row r="36" spans="1:58" s="35" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
@@ -7258,12 +7115,8 @@
       <c r="BD36" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE36" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF36" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE36" s="26"/>
+      <c r="BF36" s="26"/>
     </row>
     <row r="37" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
@@ -7434,12 +7287,8 @@
       <c r="BD37" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE37" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF37" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE37" s="26"/>
+      <c r="BF37" s="26"/>
     </row>
     <row r="38" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
@@ -7610,12 +7459,8 @@
       <c r="BD38" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE38" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF38" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE38" s="26"/>
+      <c r="BF38" s="26"/>
     </row>
     <row r="39" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
@@ -7786,12 +7631,8 @@
       <c r="BD39" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE39" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF39" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE39" s="26"/>
+      <c r="BF39" s="26"/>
     </row>
     <row r="40" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
@@ -7962,12 +7803,8 @@
       <c r="BD40" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE40" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF40" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE40" s="26"/>
+      <c r="BF40" s="26"/>
     </row>
     <row r="41" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
@@ -8138,12 +7975,8 @@
       <c r="BD41" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE41" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF41" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE41" s="26"/>
+      <c r="BF41" s="26"/>
     </row>
     <row r="42" spans="1:58" s="35" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
@@ -8314,12 +8147,8 @@
       <c r="BD42" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE42" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BF42" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE42" s="26"/>
+      <c r="BF42" s="26"/>
     </row>
     <row r="43" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
@@ -8490,12 +8319,8 @@
       <c r="BD43" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE43" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF43" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE43" s="26"/>
+      <c r="BF43" s="26"/>
     </row>
     <row r="44" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="36" t="s">
@@ -8666,12 +8491,8 @@
       <c r="BD44" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE44" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF44" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE44" s="26"/>
+      <c r="BF44" s="26"/>
     </row>
     <row r="45" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
@@ -8842,12 +8663,8 @@
       <c r="BD45" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE45" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF45" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE45" s="26"/>
+      <c r="BF45" s="26"/>
     </row>
     <row r="46" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="25" t="s">
@@ -9018,12 +8835,8 @@
       <c r="BD46" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE46" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF46" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE46" s="26"/>
+      <c r="BF46" s="26"/>
     </row>
     <row r="47" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="25" t="s">
@@ -9194,12 +9007,8 @@
       <c r="BD47" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE47" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF47" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE47" s="26"/>
+      <c r="BF47" s="26"/>
     </row>
     <row r="48" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="25" t="s">
@@ -9370,12 +9179,8 @@
       <c r="BD48" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE48" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF48" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE48" s="26"/>
+      <c r="BF48" s="26"/>
     </row>
     <row r="49" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="25" t="s">
@@ -9546,12 +9351,8 @@
       <c r="BD49" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE49" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF49" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE49" s="26"/>
+      <c r="BF49" s="26"/>
     </row>
     <row r="50" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
@@ -9722,12 +9523,8 @@
       <c r="BD50" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="BE50" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF50" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE50" s="26"/>
+      <c r="BF50" s="26"/>
     </row>
     <row r="51" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="25" t="s">
@@ -9898,12 +9695,8 @@
       <c r="BD51" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE51" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF51" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE51" s="26"/>
+      <c r="BF51" s="26"/>
     </row>
     <row r="52" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
@@ -10074,12 +9867,8 @@
       <c r="BD52" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BE52" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF52" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE52" s="26"/>
+      <c r="BF52" s="26"/>
     </row>
     <row r="53" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="25" t="s">
@@ -10250,12 +10039,8 @@
       <c r="BD53" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE53" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF53" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE53" s="26"/>
+      <c r="BF53" s="26"/>
     </row>
     <row r="54" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="25" t="s">
@@ -10426,12 +10211,8 @@
       <c r="BD54" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE54" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF54" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE54" s="26"/>
+      <c r="BF54" s="26"/>
     </row>
     <row r="55" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="25" t="s">
@@ -10602,12 +10383,8 @@
       <c r="BD55" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE55" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="BF55" s="26" t="s">
-        <v>90</v>
-      </c>
+      <c r="BE55" s="26"/>
+      <c r="BF55" s="26"/>
     </row>
     <row r="56" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="25" t="s">
@@ -10778,12 +10555,8 @@
       <c r="BD56" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE56" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF56" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE56" s="26"/>
+      <c r="BF56" s="26"/>
     </row>
     <row r="57" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="25" t="s">
@@ -10954,12 +10727,8 @@
       <c r="BD57" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE57" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF57" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE57" s="26"/>
+      <c r="BF57" s="26"/>
     </row>
     <row r="58" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
@@ -11130,12 +10899,8 @@
       <c r="BD58" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE58" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF58" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE58" s="26"/>
+      <c r="BF58" s="26"/>
     </row>
     <row r="59" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
@@ -11306,12 +11071,8 @@
       <c r="BD59" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE59" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF59" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE59" s="26"/>
+      <c r="BF59" s="26"/>
     </row>
     <row r="60" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
@@ -11482,12 +11243,8 @@
       <c r="BD60" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE60" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF60" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE60" s="26"/>
+      <c r="BF60" s="26"/>
     </row>
     <row r="61" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
@@ -11658,12 +11415,8 @@
       <c r="BD61" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE61" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF61" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE61" s="26"/>
+      <c r="BF61" s="26"/>
     </row>
     <row r="62" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
@@ -11834,12 +11587,8 @@
       <c r="BD62" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE62" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF62" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE62" s="26"/>
+      <c r="BF62" s="26"/>
     </row>
     <row r="63" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
@@ -12010,12 +11759,8 @@
       <c r="BD63" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE63" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF63" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE63" s="26"/>
+      <c r="BF63" s="26"/>
     </row>
     <row r="64" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
@@ -12186,12 +11931,8 @@
       <c r="BD64" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE64" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF64" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE64" s="26"/>
+      <c r="BF64" s="26"/>
     </row>
     <row r="65" spans="1:58" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="25" t="s">
@@ -12362,12 +12103,8 @@
       <c r="BD65" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="BE65" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF65" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="BE65" s="26"/>
+      <c r="BF65" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>